<commit_message>
Finish mark red and print people that should be kicked.
</commit_message>
<xml_diff>
--- a/6k萌新群成员段位及课题完成情况 2019.12.9.xlsx
+++ b/6k萌新群成员段位及课题完成情况 2019.12.9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\PycharmProjects\Attendence_Record\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5318D552-E035-46D3-935E-BDD20BF7A43D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA33236B-50EC-4BE2-8171-70E092EE4A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="24090" windowHeight="11385" xr2:uid="{B7F9FF18-6E5E-4E73-BF5C-BB9286558977}"/>
+    <workbookView xWindow="2820" yWindow="510" windowWidth="24090" windowHeight="11385" xr2:uid="{B7F9FF18-6E5E-4E73-BF5C-BB9286558977}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="88">
   <si>
     <t>群成员QQ号</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -398,6 +398,11 @@
   <si>
     <t>第四期课题 
 2019.9.1-2019.9.14</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第11期课题 
+2019.12.9-2019.12.22</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -825,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72770742-A439-487A-AB59-48EB2014F46E}">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -846,10 +851,11 @@
     <col min="12" max="12" width="24.5" style="1" customWidth="1"/>
     <col min="13" max="13" width="26.5" style="1" customWidth="1"/>
     <col min="14" max="15" width="20.25" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.625" style="1"/>
+    <col min="16" max="16" width="24.5" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -895,8 +901,11 @@
       <c r="O1" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>704187028</v>
       </c>
@@ -925,7 +934,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1959935816</v>
       </c>
@@ -951,7 +960,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>29012207</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>768754163</v>
       </c>
@@ -1012,7 +1021,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>932981410</v>
       </c>
@@ -1035,7 +1044,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1093596466</v>
       </c>
@@ -1058,7 +1067,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>630153499</v>
       </c>
@@ -1105,7 +1114,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2780342119</v>
       </c>
@@ -1128,7 +1137,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2423687932</v>
       </c>
@@ -1148,7 +1157,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2602236644</v>
       </c>
@@ -1177,7 +1186,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>869347974</v>
       </c>
@@ -1212,7 +1221,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1181288954</v>
       </c>
@@ -1235,7 +1244,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>772743795</v>
       </c>
@@ -1264,7 +1273,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>97490133</v>
       </c>
@@ -1296,7 +1305,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2473108024</v>
       </c>

</xml_diff>